<commit_message>
Add penalty and upcountry changes in invoice
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-upcountry-v4.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-upcountry-v4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
   <si>
     <t xml:space="preserve">ANNEXURE</t>
   </si>
@@ -145,6 +145,9 @@
     <t xml:space="preserve">{booking:rating_stars}</t>
   </si>
   <si>
+    <t xml:space="preserve">Upcountry Details</t>
+  </si>
+  <si>
     <t xml:space="preserve">Upcountry Rate</t>
   </si>
   <si>
@@ -157,7 +160,7 @@
     <t xml:space="preserve">{upcountry:booking}</t>
   </si>
   <si>
-    <t xml:space="preserve">{upcountry:upcountry_rate} PER KM</t>
+    <t xml:space="preserve">{upcountry:sf_upcountry_rate} PER KM</t>
   </si>
   <si>
     <t xml:space="preserve">{upcountry:upcountry_distance} KM</t>
@@ -166,6 +169,30 @@
     <t xml:space="preserve">{upcountry:upcountry_price}</t>
   </si>
   <si>
+    <t xml:space="preserve">Penalty Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penalty Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{penalty:booking_id}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{penalty:penalty_times}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{penalty:penalty_amount}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{penalty:p_amount}</t>
+  </si>
+  <si>
     <t xml:space="preserve">Royalty Invoice</t>
   </si>
   <si>
@@ -199,7 +226,10 @@
     <t xml:space="preserve">{meta:total_upcountry_price}</t>
   </si>
   <si>
-    <t xml:space="preserve">{meta:upcountry_st}</t>
+    <t xml:space="preserve">Total Penalty </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{meta:total_penalty_amount}</t>
   </si>
   <si>
     <t xml:space="preserve">Amount To Be Paid By 247around</t>
@@ -777,15 +807,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,20 +1188,14 @@
       <c r="M18" s="10"/>
       <c r="N18" s="13"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>43</v>
-      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
@@ -1184,34 +1208,42 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="37"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
+      <c r="B21" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>48</v>
+      </c>
       <c r="F21" s="36"/>
       <c r="G21" s="36"/>
       <c r="H21" s="36"/>
@@ -1224,279 +1256,281 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
-      <c r="B22" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="34"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="37"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="37"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1"/>
+      <c r="B24" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="L24" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="M24" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="N24" s="42" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="37"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="44" t="s">
+      <c r="B25" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="K25" s="45" t="s">
+      <c r="D25" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="L25" s="45" t="s">
+      <c r="E25" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="M25" s="45" t="s">
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="37"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="B26" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="N25" s="46" t="s">
+      <c r="C26" s="34" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1"/>
-      <c r="B26" s="47" t="s">
+      <c r="D26" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="35" t="s">
+      <c r="E26" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="13"/>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="37"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="J27" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="K27" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35"/>
-      <c r="N27" s="50"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="37"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
-      <c r="B28" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="K28" s="52"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
+      <c r="B28" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="53"/>
-      <c r="N29" s="53"/>
+      <c r="B29" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="M30" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="N30" s="42" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
-      <c r="B31" s="54" t="s">
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="K31" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="L31" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="M31" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="54"/>
-      <c r="M31" s="54"/>
-      <c r="N31" s="54"/>
+      <c r="N31" s="46" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
-      <c r="B32" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="52" t="s">
+      <c r="B32" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="52"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1"/>
-      <c r="B33" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="55"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="52" t="s">
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="52"/>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J33" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="50"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1"/>
-      <c r="B34" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="55"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="52" t="s">
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
+      <c r="J34" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="50"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
-      <c r="B35" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="52" t="s">
+      <c r="B35" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="H35" s="52"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="52"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="52" t="s">
+        <v>71</v>
+      </c>
       <c r="K35" s="52"/>
       <c r="L35" s="52"/>
       <c r="M35" s="52"/>
@@ -1504,44 +1538,174 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
-      <c r="B36" s="57" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="53"/>
+      <c r="M36" s="53"/>
+      <c r="N36" s="53"/>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="43"/>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1"/>
+      <c r="B38" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="54"/>
+      <c r="L38" s="54"/>
+      <c r="M38" s="54"/>
+      <c r="N38" s="54"/>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1"/>
+      <c r="B39" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="H39" s="52"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="52"/>
+      <c r="M39" s="52"/>
+      <c r="N39" s="52"/>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1"/>
+      <c r="B40" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="H40" s="52"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="52"/>
+      <c r="M40" s="52"/>
+      <c r="N40" s="52"/>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1"/>
+      <c r="B41" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="56"/>
+      <c r="G41" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="H41" s="52"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="52"/>
+      <c r="L41" s="52"/>
+      <c r="M41" s="52"/>
+      <c r="N41" s="52"/>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1"/>
+      <c r="B42" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="H42" s="52"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="52"/>
+      <c r="L42" s="52"/>
+      <c r="M42" s="52"/>
+      <c r="N42" s="52"/>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1"/>
+      <c r="B43" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B22:N22"/>
-    <mergeCell ref="B23:N23"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="B30:N30"/>
-    <mergeCell ref="B31:N31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="G32:N32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="G33:N33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="G34:N34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="G35:N35"/>
+    <mergeCell ref="B28:N28"/>
+    <mergeCell ref="B29:N29"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="J35:N35"/>
     <mergeCell ref="B36:I36"/>
+    <mergeCell ref="J36:N36"/>
+    <mergeCell ref="B37:N37"/>
+    <mergeCell ref="B38:N38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="G39:N39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="G40:N40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="G41:N41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="G42:N42"/>
+    <mergeCell ref="B43:I43"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Penalty Removed from invoice
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-upcountry-v4.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-upcountry-v4.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anujaggarwal/Downloads/templates/anuj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-aws/application/controllers/excel-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="90">
   <si>
     <t>ANNEXURE</t>
   </si>
@@ -158,9 +158,6 @@
     <t>{upcountry:upcountry_price}</t>
   </si>
   <si>
-    <t>Penalty Details</t>
-  </si>
-  <si>
     <t>{penalty:booking_id}</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
   </si>
   <si>
     <t>{meta:total_upcountry_price}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Penalty </t>
   </si>
   <si>
     <t>{meta:total_penalty_amount}</t>
@@ -288,6 +282,33 @@
   </si>
   <si>
     <t>Penalty Count</t>
+  </si>
+  <si>
+    <t>Penalty Applied</t>
+  </si>
+  <si>
+    <t>Penalty Removed</t>
+  </si>
+  <si>
+    <t>{cr_penalty:booking_id}</t>
+  </si>
+  <si>
+    <t>{cr_penalty:penalty_times}</t>
+  </si>
+  <si>
+    <t>{cr_penalty:penalty_amount}</t>
+  </si>
+  <si>
+    <t>{cr_penalty:p_amount}</t>
+  </si>
+  <si>
+    <t>Total Penalty Applied</t>
+  </si>
+  <si>
+    <t>Total Penalty Removed</t>
+  </si>
+  <si>
+    <t>{meta:cr_total_penalty_amount}</t>
   </si>
 </sst>
 </file>
@@ -353,7 +374,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,6 +393,12 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -668,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -823,7 +850,82 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -850,33 +952,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -889,43 +964,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1205,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="B41" sqref="B41:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1243,21 +1282,21 @@
     </row>
     <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1497,21 +1536,21 @@
     </row>
     <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
-      <c r="B16" s="66" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="68"/>
+      <c r="B16" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="76"/>
+      <c r="N16" s="77"/>
     </row>
     <row r="17" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
@@ -1525,22 +1564,22 @@
         <v>17</v>
       </c>
       <c r="E17" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="H17" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="I17" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="28" t="s">
+      <c r="J17" s="28" t="s">
         <v>75</v>
-      </c>
-      <c r="I17" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="J17" s="28" t="s">
-        <v>77</v>
       </c>
       <c r="K17" s="36" t="s">
         <v>20</v>
@@ -1631,21 +1670,21 @@
     </row>
     <row r="21" spans="1:14" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="67"/>
-      <c r="M21" s="67"/>
-      <c r="N21" s="68"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="76"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="77"/>
     </row>
     <row r="22" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
@@ -1653,10 +1692,10 @@
         <v>15</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E22" s="30" t="s">
         <v>22</v>
@@ -1729,59 +1768,59 @@
     </row>
     <row r="26" spans="1:14" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
-      <c r="B26" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="67"/>
-      <c r="J26" s="67"/>
-      <c r="K26" s="67"/>
-      <c r="L26" s="67"/>
-      <c r="M26" s="67"/>
-      <c r="N26" s="68"/>
+      <c r="B26" s="75" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="76"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="76"/>
+      <c r="N26" s="77"/>
     </row>
     <row r="27" spans="1:14" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="36" t="s">
-        <v>82</v>
+      <c r="C27" s="52" t="s">
+        <v>80</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E27" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
       <c r="N27" s="29"/>
     </row>
     <row r="28" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
       <c r="B28" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="D28" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="E28" s="33" t="s">
         <v>45</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>46</v>
       </c>
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
@@ -1811,386 +1850,507 @@
     </row>
     <row r="30" spans="1:14" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
-      <c r="B30" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="64"/>
-      <c r="L30" s="64"/>
-      <c r="M30" s="64"/>
-      <c r="N30" s="64"/>
-    </row>
-    <row r="31" spans="1:14" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="90" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="90"/>
+    </row>
+    <row r="31" spans="1:14" ht="28" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
-      <c r="B31" s="65" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="65"/>
-      <c r="M31" s="65"/>
-      <c r="N31" s="65"/>
-    </row>
-    <row r="32" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="B31" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="29"/>
+    </row>
+    <row r="32" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="49"/>
+      <c r="B32" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="47"/>
     </row>
     <row r="33" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" s="61"/>
-      <c r="J33" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="K33" s="61"/>
-      <c r="L33" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="M33" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="N33" s="29" t="s">
-        <v>22</v>
-      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="15"/>
     </row>
     <row r="34" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="I34" s="62"/>
-      <c r="J34" s="62" t="s">
-        <v>50</v>
-      </c>
-      <c r="K34" s="62"/>
-      <c r="L34" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="M34" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="N34" s="50" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="B34" s="12"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="15"/>
+    </row>
+    <row r="35" spans="1:14" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
-      <c r="B35" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="72" t="s">
-        <v>55</v>
-      </c>
+      <c r="B35" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="73"/>
       <c r="I35" s="73"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="20"/>
-    </row>
-    <row r="36" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="J35" s="73"/>
+      <c r="K35" s="73"/>
+      <c r="L35" s="73"/>
+      <c r="M35" s="73"/>
+      <c r="N35" s="73"/>
+    </row>
+    <row r="36" spans="1:14" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
-      <c r="B36" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="72" t="s">
-        <v>57</v>
-      </c>
-      <c r="I36" s="73"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="38"/>
-      <c r="L36" s="38"/>
-      <c r="M36" s="38"/>
-      <c r="N36" s="51"/>
+      <c r="B36" s="74" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="74"/>
+      <c r="K36" s="74"/>
+      <c r="L36" s="74"/>
+      <c r="M36" s="74"/>
+      <c r="N36" s="74"/>
     </row>
     <row r="37" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
-      <c r="B37" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="72" t="s">
-        <v>59</v>
-      </c>
-      <c r="I37" s="73"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="38"/>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
-      <c r="N37" s="51"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="49"/>
     </row>
     <row r="38" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
-      <c r="B38" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="74" t="s">
-        <v>61</v>
-      </c>
-      <c r="I38" s="75"/>
-      <c r="J38" s="75"/>
-      <c r="K38" s="75"/>
-      <c r="L38" s="75"/>
-      <c r="M38" s="75"/>
-      <c r="N38" s="76"/>
+      <c r="B38" s="78"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="79"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="59"/>
+      <c r="J38" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38" s="59"/>
+      <c r="L38" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="M38" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="N38" s="29" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="39" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
-      <c r="B39" s="69"/>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
-      <c r="G39" s="69"/>
-      <c r="H39" s="69"/>
-      <c r="I39" s="69"/>
-      <c r="J39" s="70"/>
-      <c r="K39" s="70"/>
-      <c r="L39" s="70"/>
-      <c r="M39" s="70"/>
-      <c r="N39" s="71"/>
+      <c r="B39" s="83"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="84"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="I39" s="60"/>
+      <c r="J39" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="K39" s="60"/>
+      <c r="L39" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="M39" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="N39" s="50" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="40" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
-      <c r="B40" s="69"/>
-      <c r="C40" s="69"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="69"/>
-      <c r="G40" s="69"/>
-      <c r="H40" s="69"/>
-      <c r="I40" s="69"/>
-      <c r="J40" s="69"/>
-      <c r="K40" s="69"/>
-      <c r="L40" s="69"/>
-      <c r="M40" s="69"/>
-      <c r="N40" s="77"/>
-    </row>
-    <row r="41" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B40" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="82"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="82"/>
+      <c r="F40" s="82"/>
+      <c r="G40" s="82"/>
+      <c r="H40" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" s="89"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="38"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="20"/>
+    </row>
+    <row r="41" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
-      <c r="B41" s="79" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" s="62"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="62"/>
-      <c r="G41" s="62"/>
-      <c r="H41" s="62"/>
-      <c r="I41" s="62"/>
-      <c r="J41" s="62"/>
-      <c r="K41" s="62"/>
-      <c r="L41" s="62"/>
-      <c r="M41" s="62"/>
-      <c r="N41" s="80"/>
+      <c r="B41" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="82"/>
+      <c r="D41" s="82"/>
+      <c r="E41" s="82"/>
+      <c r="F41" s="82"/>
+      <c r="G41" s="82"/>
+      <c r="H41" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="I41" s="89"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="38"/>
+      <c r="N41" s="51"/>
     </row>
     <row r="42" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="B42" s="81" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78"/>
-      <c r="G42" s="62" t="s">
-        <v>64</v>
-      </c>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="62"/>
-      <c r="K42" s="62"/>
-      <c r="L42" s="62"/>
-      <c r="M42" s="62"/>
-      <c r="N42" s="80"/>
+        <v>87</v>
+      </c>
+      <c r="C42" s="82"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="82"/>
+      <c r="G42" s="82"/>
+      <c r="H42" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="I42" s="89"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="51"/>
     </row>
     <row r="43" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
       <c r="B43" s="81" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="61"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="78"/>
-      <c r="G43" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="H43" s="62"/>
-      <c r="I43" s="62"/>
-      <c r="J43" s="62"/>
-      <c r="K43" s="62"/>
-      <c r="L43" s="62"/>
-      <c r="M43" s="62"/>
-      <c r="N43" s="80"/>
+        <v>88</v>
+      </c>
+      <c r="C43" s="82"/>
+      <c r="D43" s="82"/>
+      <c r="E43" s="82"/>
+      <c r="F43" s="82"/>
+      <c r="G43" s="82"/>
+      <c r="H43" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="I43" s="88"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="53"/>
+      <c r="L43" s="53"/>
+      <c r="M43" s="53"/>
+      <c r="N43" s="51"/>
     </row>
     <row r="44" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="B44" s="81" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
-      <c r="G44" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="H44" s="62"/>
-      <c r="I44" s="62"/>
-      <c r="J44" s="62"/>
-      <c r="K44" s="62"/>
-      <c r="L44" s="62"/>
-      <c r="M44" s="62"/>
-      <c r="N44" s="80"/>
-    </row>
-    <row r="45" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="C44" s="82"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="82"/>
+      <c r="G44" s="82"/>
+      <c r="H44" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="I44" s="67"/>
+      <c r="J44" s="67"/>
+      <c r="K44" s="67"/>
+      <c r="L44" s="67"/>
+      <c r="M44" s="67"/>
+      <c r="N44" s="68"/>
+    </row>
+    <row r="45" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
-      <c r="B45" s="82" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" s="83"/>
-      <c r="D45" s="83"/>
-      <c r="E45" s="84"/>
-      <c r="F45" s="84"/>
-      <c r="G45" s="85" t="s">
-        <v>70</v>
-      </c>
-      <c r="H45" s="85"/>
-      <c r="I45" s="85"/>
-      <c r="J45" s="85"/>
-      <c r="K45" s="85"/>
-      <c r="L45" s="85"/>
-      <c r="M45" s="85"/>
-      <c r="N45" s="86"/>
+      <c r="B45" s="69"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
+      <c r="H45" s="69"/>
+      <c r="I45" s="69"/>
+      <c r="J45" s="86"/>
+      <c r="K45" s="86"/>
+      <c r="L45" s="86"/>
+      <c r="M45" s="86"/>
+      <c r="N45" s="87"/>
     </row>
     <row r="46" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
-      <c r="B46" s="52"/>
-      <c r="C46" s="52"/>
-      <c r="D46" s="52"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="52"/>
-      <c r="H46" s="52"/>
-      <c r="I46" s="52"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-    </row>
-    <row r="47" spans="1:14" ht="14" x14ac:dyDescent="0.15">
-      <c r="B47" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="52"/>
-      <c r="F47" s="52"/>
-      <c r="G47" s="52"/>
-      <c r="H47" s="52"/>
-      <c r="I47" s="52"/>
-      <c r="J47" s="52"/>
-      <c r="K47" s="52"/>
-      <c r="L47" s="52"/>
-      <c r="M47" s="52"/>
-      <c r="N47" s="52"/>
+      <c r="B46" s="69"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="69"/>
+      <c r="I46" s="69"/>
+      <c r="J46" s="69"/>
+      <c r="K46" s="69"/>
+      <c r="L46" s="69"/>
+      <c r="M46" s="69"/>
+      <c r="N46" s="70"/>
+    </row>
+    <row r="47" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="1"/>
+      <c r="B47" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" s="60"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="60"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="60"/>
+      <c r="I47" s="60"/>
+      <c r="J47" s="60"/>
+      <c r="K47" s="60"/>
+      <c r="L47" s="60"/>
+      <c r="M47" s="60"/>
+      <c r="N47" s="61"/>
+    </row>
+    <row r="48" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="A48" s="1"/>
+      <c r="B48" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" s="59"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="H48" s="60"/>
+      <c r="I48" s="60"/>
+      <c r="J48" s="60"/>
+      <c r="K48" s="60"/>
+      <c r="L48" s="60"/>
+      <c r="M48" s="60"/>
+      <c r="N48" s="61"/>
+    </row>
+    <row r="49" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="A49" s="1"/>
+      <c r="B49" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" s="60"/>
+      <c r="I49" s="60"/>
+      <c r="J49" s="60"/>
+      <c r="K49" s="60"/>
+      <c r="L49" s="60"/>
+      <c r="M49" s="60"/>
+      <c r="N49" s="61"/>
+    </row>
+    <row r="50" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="A50" s="1"/>
+      <c r="B50" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="H50" s="60"/>
+      <c r="I50" s="60"/>
+      <c r="J50" s="60"/>
+      <c r="K50" s="60"/>
+      <c r="L50" s="60"/>
+      <c r="M50" s="60"/>
+      <c r="N50" s="61"/>
+    </row>
+    <row r="51" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="63"/>
+      <c r="D51" s="63"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="H51" s="64"/>
+      <c r="I51" s="64"/>
+      <c r="J51" s="64"/>
+      <c r="K51" s="64"/>
+      <c r="L51" s="64"/>
+      <c r="M51" s="64"/>
+      <c r="N51" s="65"/>
+    </row>
+    <row r="52" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="A52" s="1"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+    </row>
+    <row r="53" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="B53" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="57"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="57"/>
+      <c r="J53" s="57"/>
+      <c r="K53" s="57"/>
+      <c r="L53" s="57"/>
+      <c r="M53" s="57"/>
+      <c r="N53" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="B46:I46"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="G43:N43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="G44:N44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="G45:N45"/>
-    <mergeCell ref="H38:N38"/>
-    <mergeCell ref="B40:N40"/>
-    <mergeCell ref="B41:N41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="G42:N42"/>
+  <mergeCells count="37">
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="B53:N53"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="J45:N45"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
     <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B30:N30"/>
-    <mergeCell ref="B31:N31"/>
+    <mergeCell ref="B35:N35"/>
+    <mergeCell ref="B36:N36"/>
     <mergeCell ref="B16:N16"/>
     <mergeCell ref="B21:N21"/>
     <mergeCell ref="B26:N26"/>
+    <mergeCell ref="B30:N30"/>
+    <mergeCell ref="H44:N44"/>
+    <mergeCell ref="B46:N46"/>
     <mergeCell ref="B47:N47"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="B39:I39"/>
-    <mergeCell ref="J39:N39"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="G48:N48"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="G49:N49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="G50:N50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="G51:N51"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>